<commit_message>
Conv layer is added completely
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t xml:space="preserve">4 block, each block 2 Conv, the second would be normal/resconv., 128,128,24</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t xml:space="preserve"># of Filters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stream</t>
   </si>
   <si>
     <t xml:space="preserve">Precision</t>
@@ -123,7 +120,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,8 +129,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBEE3D3"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <fgColor rgb="FF59C5C7"/>
+        <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -145,13 +142,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFBEE3D3"/>
+        <bgColor rgb="FFFCD4D1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFDC578"/>
         <bgColor rgb="FFF7A19A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBCE4E5"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD4D1"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -170,12 +179,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF04E4D"/>
         <bgColor rgb="FF993366"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFCD4D1"/>
-        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -226,7 +229,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -315,31 +318,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -388,14 +395,14 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFBEE3D3"/>
+      <rgbColor rgb="FFBCE4E5"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFF7A19A"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFDC578"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF59C5C7"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
@@ -967,58 +974,58 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N16" activeCellId="0" sqref="N16"/>
+      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="0" width="6.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="15" style="0" width="5.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="12" width="5.04"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="6.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="14" style="0" width="5.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="12" width="5.04"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1" s="13"/>
-      <c r="G1" s="14" t="s">
+      <c r="C1" s="13"/>
+      <c r="F1" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="G1" s="14"/>
       <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="K1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>16</v>
       </c>
+      <c r="K1" s="15"/>
       <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="O1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>17</v>
       </c>
+      <c r="O1" s="16"/>
       <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="13"/>
-      <c r="G2" s="14" t="s">
+      <c r="C2" s="13"/>
+      <c r="F2" s="14" t="s">
         <v>18</v>
       </c>
+      <c r="G2" s="14"/>
       <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="K2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>18</v>
       </c>
+      <c r="K2" s="15"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="O2" s="16" t="s">
+      <c r="N2" s="16" t="s">
         <v>18</v>
       </c>
+      <c r="O2" s="16"/>
       <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
@@ -1027,51 +1034,48 @@
       <c r="B3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>22</v>
-      </c>
+      <c r="D3" s="18"/>
       <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="F3" s="19" t="n">
+        <v>64</v>
+      </c>
       <c r="G3" s="19" t="n">
+        <v>96</v>
+      </c>
+      <c r="H3" s="19" t="n">
+        <v>128</v>
+      </c>
+      <c r="J3" s="20" t="n">
         <v>64</v>
       </c>
-      <c r="H3" s="19" t="n">
+      <c r="K3" s="20" t="n">
         <v>96</v>
       </c>
-      <c r="I3" s="19" t="n">
+      <c r="L3" s="20" t="n">
         <v>128</v>
       </c>
-      <c r="K3" s="20" t="n">
+      <c r="N3" s="21" t="n">
         <v>64</v>
       </c>
-      <c r="L3" s="20" t="n">
+      <c r="O3" s="21" t="n">
         <v>96</v>
       </c>
-      <c r="M3" s="20" t="n">
-        <v>128</v>
-      </c>
-      <c r="O3" s="21" t="n">
-        <v>64</v>
-      </c>
       <c r="P3" s="21" t="n">
-        <v>96</v>
-      </c>
-      <c r="Q3" s="21" t="n">
         <v>128</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B4" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="17" t="n">
         <v>2</v>
-      </c>
-      <c r="B4" s="17" t="n">
-        <v>16</v>
-      </c>
-      <c r="C4" s="17" t="n">
-        <v>3</v>
       </c>
       <c r="D4" s="17" t="n">
         <v>2</v>
@@ -1079,277 +1083,262 @@
       <c r="E4" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="17" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="19" t="n">
+      <c r="F4" s="22" t="n">
         <v>811</v>
       </c>
-      <c r="H4" s="19" t="n">
+      <c r="G4" s="22" t="n">
         <v>1162</v>
       </c>
-      <c r="I4" s="19" t="n">
+      <c r="H4" s="22" t="n">
         <v>1342</v>
       </c>
-      <c r="K4" s="22" t="n">
-        <f aca="false">C4*D4*D5*B4*A4</f>
+      <c r="J4" s="23" t="n">
+        <f aca="false">B4*C4*C5*A4</f>
+        <v>6144</v>
+      </c>
+      <c r="K4" s="23" t="n">
+        <f aca="false">B4*D4*D5*A4</f>
+        <v>9216</v>
+      </c>
+      <c r="L4" s="23" t="n">
+        <f aca="false">B4*E4*E5*A4</f>
         <v>12288</v>
       </c>
-      <c r="L4" s="22" t="n">
-        <f aca="false">C4*E4*E5*B4*A4</f>
-        <v>18432</v>
-      </c>
-      <c r="M4" s="22" t="n">
-        <f aca="false">C4*F4*F5*B4*A4</f>
-        <v>24576</v>
-      </c>
-      <c r="O4" s="23" t="n">
+      <c r="N4" s="24" t="n">
+        <f aca="false">F4/J4</f>
+        <v>0.131998697916667</v>
+      </c>
+      <c r="O4" s="24" t="n">
         <f aca="false">G4/K4</f>
-        <v>0.0659993489583333</v>
-      </c>
-      <c r="P4" s="23" t="n">
+        <v>0.126085069444444</v>
+      </c>
+      <c r="P4" s="24" t="n">
         <f aca="false">H4/L4</f>
-        <v>0.0630425347222222</v>
-      </c>
-      <c r="Q4" s="23" t="n">
-        <f aca="false">I4/M4</f>
-        <v>0.0546061197916667</v>
-      </c>
-      <c r="R4" s="12" t="n">
-        <f aca="false">AVERAGE(O4:Q4)</f>
-        <v>0.0612160011574074</v>
+        <v>0.109212239583333</v>
+      </c>
+      <c r="Q4" s="12" t="n">
+        <f aca="false">AVERAGE(N4:P4)</f>
+        <v>0.122432002314815</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B5" s="17" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C5" s="17" t="n">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="D5" s="17" t="n">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="E5" s="17" t="n">
-        <v>96</v>
-      </c>
-      <c r="F5" s="17" t="n">
         <v>128</v>
       </c>
-      <c r="G5" s="19" t="n">
+      <c r="F5" s="22" t="n">
         <v>27062</v>
       </c>
-      <c r="H5" s="19" t="n">
+      <c r="G5" s="22" t="n">
         <v>56646</v>
       </c>
-      <c r="I5" s="19" t="n">
+      <c r="H5" s="22" t="n">
         <v>90907</v>
       </c>
-      <c r="K5" s="22" t="n">
-        <f aca="false">C5*D5*D6*B5*A5</f>
+      <c r="J5" s="23" t="n">
+        <f aca="false">B5*C5*C6*A5</f>
         <v>196608</v>
       </c>
-      <c r="L5" s="22" t="n">
-        <f aca="false">C5*E5*E6*B5*A5</f>
+      <c r="K5" s="23" t="n">
+        <f aca="false">B5*D5*D6*A5</f>
         <v>442368</v>
       </c>
-      <c r="M5" s="22" t="n">
-        <f aca="false">C5*F5*F6*B5*A5</f>
+      <c r="L5" s="23" t="n">
+        <f aca="false">B5*E5*E6*A5</f>
         <v>786432</v>
       </c>
-      <c r="O5" s="24" t="n">
+      <c r="N5" s="25" t="n">
+        <f aca="false">F5/J5</f>
+        <v>0.137644449869792</v>
+      </c>
+      <c r="O5" s="25" t="n">
         <f aca="false">G5/K5</f>
-        <v>0.137644449869792</v>
-      </c>
-      <c r="P5" s="24" t="n">
+        <v>0.1280517578125</v>
+      </c>
+      <c r="P5" s="25" t="n">
         <f aca="false">H5/L5</f>
-        <v>0.1280517578125</v>
-      </c>
-      <c r="Q5" s="24" t="n">
-        <f aca="false">I5/M5</f>
         <v>0.115594228108724</v>
       </c>
-      <c r="R5" s="12" t="n">
-        <f aca="false">AVERAGE(O5:Q5)</f>
+      <c r="Q5" s="12" t="n">
+        <f aca="false">AVERAGE(N5:P5)</f>
         <v>0.127096811930339</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B6" s="17" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C6" s="17" t="n">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="D6" s="17" t="n">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="E6" s="17" t="n">
-        <v>96</v>
-      </c>
-      <c r="F6" s="17" t="n">
         <v>128</v>
       </c>
-      <c r="G6" s="19" t="n">
+      <c r="F6" s="22" t="n">
         <v>12672</v>
       </c>
-      <c r="H6" s="19" t="n">
+      <c r="G6" s="22" t="n">
         <v>28486</v>
       </c>
-      <c r="I6" s="19" t="n">
+      <c r="H6" s="22" t="n">
         <v>48791</v>
       </c>
-      <c r="K6" s="22" t="n">
-        <f aca="false">C6*D6*D7*B6*A6</f>
+      <c r="J6" s="23" t="n">
+        <f aca="false">B6*C6*C7*A6</f>
         <v>98304</v>
       </c>
-      <c r="L6" s="22" t="n">
-        <f aca="false">C6*E6*E7*B6*A6</f>
+      <c r="K6" s="23" t="n">
+        <f aca="false">B6*D6*D7*A6</f>
         <v>221184</v>
       </c>
-      <c r="M6" s="22" t="n">
-        <f aca="false">C6*F6*F7*B6*A6</f>
+      <c r="L6" s="23" t="n">
+        <f aca="false">B6*E6*E7*A6</f>
         <v>393216</v>
       </c>
-      <c r="O6" s="24" t="n">
+      <c r="N6" s="25" t="n">
+        <f aca="false">F6/J6</f>
+        <v>0.12890625</v>
+      </c>
+      <c r="O6" s="25" t="n">
         <f aca="false">G6/K6</f>
-        <v>0.12890625</v>
-      </c>
-      <c r="P6" s="24" t="n">
+        <v>0.128788700810185</v>
+      </c>
+      <c r="P6" s="25" t="n">
         <f aca="false">H6/L6</f>
-        <v>0.128788700810185</v>
-      </c>
-      <c r="Q6" s="24" t="n">
-        <f aca="false">I6/M6</f>
         <v>0.12408192952474</v>
       </c>
-      <c r="R6" s="12" t="n">
-        <f aca="false">AVERAGE(O6:Q6)</f>
+      <c r="Q6" s="12" t="n">
+        <f aca="false">AVERAGE(N6:P6)</f>
         <v>0.127258960111642</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B7" s="17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="17" t="n">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="D7" s="17" t="n">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="E7" s="17" t="n">
-        <v>96</v>
-      </c>
-      <c r="F7" s="17" t="n">
         <v>128</v>
       </c>
-      <c r="G7" s="19" t="n">
+      <c r="F7" s="22" t="n">
         <v>5988</v>
       </c>
-      <c r="H7" s="19" t="n">
+      <c r="G7" s="22" t="n">
         <v>13017</v>
       </c>
-      <c r="I7" s="19" t="n">
+      <c r="H7" s="22" t="n">
         <v>23369</v>
       </c>
-      <c r="K7" s="22" t="n">
-        <f aca="false">C7*D7*D8*B7*A7</f>
+      <c r="J7" s="23" t="n">
+        <f aca="false">B7*C7*C8*A7</f>
         <v>49152</v>
       </c>
-      <c r="L7" s="22" t="n">
-        <f aca="false">C7*E7*E8*B7*A7</f>
+      <c r="K7" s="23" t="n">
+        <f aca="false">B7*D7*D8*A7</f>
         <v>110592</v>
       </c>
-      <c r="M7" s="22" t="n">
-        <f aca="false">C7*F7*F8*B7*A7</f>
+      <c r="L7" s="23" t="n">
+        <f aca="false">B7*E7*E8*A7</f>
         <v>196608</v>
       </c>
-      <c r="O7" s="24" t="n">
+      <c r="N7" s="25" t="n">
+        <f aca="false">F7/J7</f>
+        <v>0.121826171875</v>
+      </c>
+      <c r="O7" s="25" t="n">
         <f aca="false">G7/K7</f>
-        <v>0.121826171875</v>
-      </c>
-      <c r="P7" s="24" t="n">
+        <v>0.117702907986111</v>
+      </c>
+      <c r="P7" s="25" t="n">
         <f aca="false">H7/L7</f>
-        <v>0.117702907986111</v>
-      </c>
-      <c r="Q7" s="24" t="n">
-        <f aca="false">I7/M7</f>
         <v>0.118860880533854</v>
       </c>
-      <c r="R7" s="12" t="n">
-        <f aca="false">AVERAGE(O7:Q7)</f>
+      <c r="Q7" s="12" t="n">
+        <f aca="false">AVERAGE(N7:P7)</f>
         <v>0.119463320131655</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="17" t="n">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="D8" s="17" t="n">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="E8" s="17" t="n">
-        <v>96</v>
-      </c>
-      <c r="F8" s="17" t="n">
         <v>128</v>
       </c>
-      <c r="G8" s="19" t="n">
+      <c r="F8" s="22" t="n">
         <v>3320</v>
       </c>
-      <c r="H8" s="19" t="n">
+      <c r="G8" s="22" t="n">
         <v>7040</v>
       </c>
-      <c r="I8" s="19" t="n">
+      <c r="H8" s="22" t="n">
         <v>13248</v>
       </c>
-      <c r="K8" s="22" t="n">
-        <f aca="false">C8*D8*D9*B8*A8</f>
+      <c r="J8" s="23" t="n">
+        <f aca="false">B8*C8*C9*A8</f>
         <v>24576</v>
       </c>
-      <c r="L8" s="22" t="n">
-        <f aca="false">C8*E8*E9*B8*A8</f>
+      <c r="K8" s="23" t="n">
+        <f aca="false">B8*D8*D9*A8</f>
         <v>55296</v>
       </c>
-      <c r="M8" s="22" t="n">
-        <f aca="false">C8*F8*F9*B8*A8</f>
+      <c r="L8" s="23" t="n">
+        <f aca="false">B8*E8*E9*A8</f>
         <v>98304</v>
       </c>
-      <c r="O8" s="24" t="n">
+      <c r="N8" s="25" t="n">
+        <f aca="false">F8/J8</f>
+        <v>0.135091145833333</v>
+      </c>
+      <c r="O8" s="25" t="n">
         <f aca="false">G8/K8</f>
-        <v>0.135091145833333</v>
-      </c>
-      <c r="P8" s="24" t="n">
+        <v>0.127314814814815</v>
+      </c>
+      <c r="P8" s="25" t="n">
         <f aca="false">H8/L8</f>
-        <v>0.127314814814815</v>
-      </c>
-      <c r="Q8" s="24" t="n">
-        <f aca="false">I8/M8</f>
         <v>0.134765625</v>
       </c>
+      <c r="Q8" s="12" t="n">
+        <f aca="false">AVERAGE(N8:P8)</f>
+        <v>0.132390528549383</v>
+      </c>
       <c r="R8" s="12" t="n">
-        <f aca="false">AVERAGE(O8:Q8)</f>
-        <v>0.132390528549383</v>
-      </c>
-      <c r="S8" s="12" t="n">
-        <f aca="false">AVERAGE(R5:R8)</f>
-        <v>0.126552405180755</v>
+        <f aca="false">AVERAGE(Q5:Q8)</f>
+        <v>0.126552405180754</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1357,55 +1346,52 @@
         <v>1</v>
       </c>
       <c r="B9" s="17" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" s="17" t="n">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="D9" s="17" t="n">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="E9" s="17" t="n">
-        <v>96</v>
-      </c>
-      <c r="F9" s="17" t="n">
         <v>128</v>
       </c>
-      <c r="G9" s="19" t="n">
+      <c r="F9" s="22" t="n">
         <v>3294</v>
       </c>
-      <c r="H9" s="19" t="n">
+      <c r="G9" s="22" t="n">
         <v>6721</v>
       </c>
-      <c r="I9" s="19" t="n">
+      <c r="H9" s="22" t="n">
         <v>11895</v>
       </c>
-      <c r="K9" s="22" t="n">
-        <f aca="false">C9*D9*D10*B9*A9</f>
+      <c r="J9" s="23" t="n">
+        <f aca="false">B9*C9*C10*A9</f>
         <v>12288</v>
       </c>
-      <c r="L9" s="22" t="n">
-        <f aca="false">C9*E9*E10*B9*A9</f>
+      <c r="K9" s="23" t="n">
+        <f aca="false">B9*D9*D10*A9</f>
         <v>27648</v>
       </c>
-      <c r="M9" s="22" t="n">
-        <f aca="false">C9*F9*F10*B9*A9</f>
+      <c r="L9" s="23" t="n">
+        <f aca="false">B9*E9*E10*A9</f>
         <v>49152</v>
       </c>
-      <c r="O9" s="25" t="n">
+      <c r="N9" s="26" t="n">
+        <f aca="false">F9/J9</f>
+        <v>0.26806640625</v>
+      </c>
+      <c r="O9" s="26" t="n">
         <f aca="false">G9/K9</f>
-        <v>0.26806640625</v>
-      </c>
-      <c r="P9" s="25" t="n">
+        <v>0.243091724537037</v>
+      </c>
+      <c r="P9" s="26" t="n">
         <f aca="false">H9/L9</f>
-        <v>0.243091724537037</v>
-      </c>
-      <c r="Q9" s="25" t="n">
-        <f aca="false">I9/M9</f>
         <v>0.24200439453125</v>
       </c>
-      <c r="R9" s="12" t="n">
-        <f aca="false">AVERAGE(O9:Q9)</f>
+      <c r="Q9" s="12" t="n">
+        <f aca="false">AVERAGE(N9:P9)</f>
         <v>0.251054175106096</v>
       </c>
     </row>
@@ -1414,382 +1400,404 @@
         <v>1</v>
       </c>
       <c r="B10" s="17" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" s="17" t="n">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="D10" s="17" t="n">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="E10" s="17" t="n">
-        <v>96</v>
-      </c>
-      <c r="F10" s="17" t="n">
         <v>128</v>
       </c>
-      <c r="G10" s="19" t="n">
+      <c r="F10" s="22" t="n">
         <v>3390</v>
       </c>
-      <c r="H10" s="19" t="n">
+      <c r="G10" s="22" t="n">
         <v>7044</v>
       </c>
-      <c r="I10" s="19" t="n">
+      <c r="H10" s="22" t="n">
         <v>12430</v>
       </c>
-      <c r="K10" s="22" t="n">
-        <f aca="false">C10*D10*D11*B10*A10</f>
+      <c r="J10" s="23" t="n">
+        <f aca="false">B10*C10*C11*A10</f>
         <v>12288</v>
       </c>
-      <c r="L10" s="22" t="n">
-        <f aca="false">C10*E10*E11*B10*A10</f>
+      <c r="K10" s="23" t="n">
+        <f aca="false">B10*D10*D11*A10</f>
         <v>27648</v>
       </c>
-      <c r="M10" s="22" t="n">
-        <f aca="false">C10*F10*F11*B10*A10</f>
+      <c r="L10" s="23" t="n">
+        <f aca="false">B10*E10*E11*A10</f>
         <v>49152</v>
       </c>
-      <c r="O10" s="25" t="n">
+      <c r="N10" s="26" t="n">
+        <f aca="false">F10/J10</f>
+        <v>0.27587890625</v>
+      </c>
+      <c r="O10" s="26" t="n">
         <f aca="false">G10/K10</f>
-        <v>0.27587890625</v>
-      </c>
-      <c r="P10" s="25" t="n">
+        <v>0.254774305555556</v>
+      </c>
+      <c r="P10" s="26" t="n">
         <f aca="false">H10/L10</f>
-        <v>0.254774305555556</v>
-      </c>
-      <c r="Q10" s="25" t="n">
-        <f aca="false">I10/M10</f>
         <v>0.252888997395833</v>
       </c>
+      <c r="Q10" s="12" t="n">
+        <f aca="false">AVERAGE(N10:P10)</f>
+        <v>0.261180736400463</v>
+      </c>
       <c r="R10" s="12" t="n">
-        <f aca="false">AVERAGE(O10:Q10)</f>
-        <v>0.261180736400463</v>
-      </c>
-      <c r="S10" s="12" t="n">
-        <f aca="false">AVERAGE(Q9:Q10)</f>
+        <f aca="false">AVERAGE(P9:P10)</f>
         <v>0.247446695963542</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
+      <c r="C11" s="17" t="n">
+        <v>64</v>
+      </c>
       <c r="D11" s="17" t="n">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="E11" s="17" t="n">
-        <v>96</v>
-      </c>
-      <c r="F11" s="17" t="n">
         <v>128</v>
       </c>
+      <c r="F11" s="19" t="n">
+        <f aca="false">SUM(F4:F10)</f>
+        <v>56537</v>
+      </c>
+      <c r="G11" s="19" t="n">
+        <f aca="false">SUM(G4:G10)</f>
+        <v>120116</v>
+      </c>
+      <c r="H11" s="19" t="n">
+        <f aca="false">SUM(H4:H10)</f>
+        <v>201982</v>
+      </c>
+      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+      <c r="N11" s="12"/>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R12" s="12"/>
+      <c r="Q12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R13" s="12"/>
+      <c r="Q13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R14" s="12"/>
+      <c r="Q14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G15" s="0" t="n">
+      <c r="F15" s="22" t="n">
         <v>3886</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="G15" s="22" t="n">
         <v>4290</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="H15" s="22" t="n">
         <v>5397</v>
       </c>
+      <c r="J15" s="0" t="n">
+        <f aca="false">A4*B4*C4*C5</f>
+        <v>6144</v>
+      </c>
       <c r="K15" s="0" t="n">
-        <f aca="false">A4*B4*C4*D4*D5</f>
+        <f aca="false">A4*B4*D4*D5</f>
+        <v>9216</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <f aca="false">A4*B4*E4*E5</f>
         <v>12288</v>
       </c>
-      <c r="L15" s="0" t="n">
-        <f aca="false">A4*B4*C4*E4*E5</f>
-        <v>18432</v>
-      </c>
-      <c r="M15" s="0" t="n">
-        <f aca="false">A4*B4*C4*F4*F5</f>
+      <c r="N15" s="27" t="n">
+        <f aca="false">F15/J15</f>
+        <v>0.632486979166667</v>
+      </c>
+      <c r="O15" s="27" t="n">
+        <f aca="false">G15/K15</f>
+        <v>0.465494791666667</v>
+      </c>
+      <c r="P15" s="27" t="n">
+        <f aca="false">H15/L15</f>
+        <v>0.439208984375</v>
+      </c>
+      <c r="Q15" s="12" t="n">
+        <f aca="false">AVERAGE(N15:P15)</f>
+        <v>0.512396918402778</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="22" t="n">
+        <v>37625</v>
+      </c>
+      <c r="G16" s="22" t="n">
+        <v>75273</v>
+      </c>
+      <c r="H16" s="22" t="n">
+        <v>122778</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <f aca="false">A5*B5*C5*C6</f>
+        <v>196608</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <f aca="false">A5*B5*D5*D6</f>
+        <v>442368</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <f aca="false">A5*B5*E5*E6</f>
+        <v>786432</v>
+      </c>
+      <c r="N16" s="28" t="n">
+        <f aca="false">F16/J16</f>
+        <v>0.191370646158854</v>
+      </c>
+      <c r="O16" s="28" t="n">
+        <f aca="false">G16/K16</f>
+        <v>0.170159233940972</v>
+      </c>
+      <c r="P16" s="28" t="n">
+        <f aca="false">H16/L16</f>
+        <v>0.156120300292969</v>
+      </c>
+      <c r="Q16" s="12" t="n">
+        <f aca="false">AVERAGE(N16:P16)</f>
+        <v>0.172550060130932</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="22" t="n">
+        <v>19512</v>
+      </c>
+      <c r="G17" s="22" t="n">
+        <v>40276</v>
+      </c>
+      <c r="H17" s="22" t="n">
+        <v>66916</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <f aca="false">A6*B6*C6*C7</f>
+        <v>98304</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <f aca="false">A6*B6*D6*D7</f>
+        <v>221184</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <f aca="false">A6*B6*E6*E7</f>
+        <v>393216</v>
+      </c>
+      <c r="N17" s="28" t="n">
+        <f aca="false">F17/J17</f>
+        <v>0.198486328125</v>
+      </c>
+      <c r="O17" s="28" t="n">
+        <f aca="false">G17/K17</f>
+        <v>0.182092737268519</v>
+      </c>
+      <c r="P17" s="28" t="n">
+        <f aca="false">H17/L17</f>
+        <v>0.170176188151042</v>
+      </c>
+      <c r="Q17" s="12" t="n">
+        <f aca="false">AVERAGE(N17:P17)</f>
+        <v>0.183585084514853</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="22" t="n">
+        <v>10093</v>
+      </c>
+      <c r="G18" s="22" t="n">
+        <v>20553</v>
+      </c>
+      <c r="H18" s="22" t="n">
+        <v>36533</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <f aca="false">A7*B7*C7*C8</f>
+        <v>49152</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <f aca="false">A7*B7*D7*D8</f>
+        <v>110592</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <f aca="false">A7*B7*E7*E8</f>
+        <v>196608</v>
+      </c>
+      <c r="N18" s="28" t="n">
+        <f aca="false">F18/J18</f>
+        <v>0.205342610677083</v>
+      </c>
+      <c r="O18" s="28" t="n">
+        <f aca="false">G18/K18</f>
+        <v>0.185845269097222</v>
+      </c>
+      <c r="P18" s="28" t="n">
+        <f aca="false">H18/L18</f>
+        <v>0.185816446940104</v>
+      </c>
+      <c r="Q18" s="12" t="n">
+        <f aca="false">AVERAGE(N18:P18)</f>
+        <v>0.19233477557147</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="22" t="n">
+        <v>5550</v>
+      </c>
+      <c r="G19" s="22" t="n">
+        <v>11667</v>
+      </c>
+      <c r="H19" s="22" t="n">
+        <v>20367</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <f aca="false">A8*B8*C8*C9</f>
         <v>24576</v>
       </c>
-      <c r="O15" s="26" t="n">
-        <f aca="false">G15/K15</f>
-        <v>0.316243489583333</v>
-      </c>
-      <c r="P15" s="26" t="n">
-        <f aca="false">H15/L15</f>
-        <v>0.232747395833333</v>
-      </c>
-      <c r="Q15" s="26" t="n">
-        <f aca="false">I15/M15</f>
-        <v>0.2196044921875</v>
-      </c>
-      <c r="R15" s="12" t="n">
-        <f aca="false">AVERAGE(O15:Q15)</f>
-        <v>0.256198459201389</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G16" s="0" t="n">
-        <v>37625</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>75273</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>122778</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <f aca="false">A5*B5*C5*D5*D6</f>
-        <v>196608</v>
-      </c>
-      <c r="L16" s="0" t="n">
-        <f aca="false">A5*B5*C5*E5*E6</f>
-        <v>442368</v>
-      </c>
-      <c r="M16" s="0" t="n">
-        <f aca="false">A5*B5*C5*F5*F6</f>
-        <v>786432</v>
-      </c>
-      <c r="O16" s="27" t="n">
-        <f aca="false">G16/K16</f>
-        <v>0.191370646158854</v>
-      </c>
-      <c r="P16" s="27" t="n">
-        <f aca="false">H16/L16</f>
-        <v>0.170159233940972</v>
-      </c>
-      <c r="Q16" s="27" t="n">
-        <f aca="false">I16/M16</f>
-        <v>0.156120300292969</v>
-      </c>
-      <c r="R16" s="12" t="n">
-        <f aca="false">AVERAGE(O16:Q16)</f>
-        <v>0.172550060130932</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G17" s="0" t="n">
-        <v>19512</v>
-      </c>
-      <c r="H17" s="0" t="n">
-        <v>40276</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <v>66916</v>
-      </c>
-      <c r="K17" s="0" t="n">
-        <f aca="false">A6*B6*C6*D6*D7</f>
+      <c r="K19" s="0" t="n">
+        <f aca="false">A8*B8*D8*D9</f>
+        <v>55296</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <f aca="false">A8*B8*E8*E9</f>
         <v>98304</v>
       </c>
-      <c r="L17" s="0" t="n">
-        <f aca="false">A6*B6*C6*E6*E7</f>
-        <v>221184</v>
-      </c>
-      <c r="M17" s="0" t="n">
-        <f aca="false">A6*B6*C6*F6*F7</f>
-        <v>393216</v>
-      </c>
-      <c r="O17" s="27" t="n">
-        <f aca="false">G17/K17</f>
-        <v>0.198486328125</v>
-      </c>
-      <c r="P17" s="27" t="n">
-        <f aca="false">H17/L17</f>
-        <v>0.182092737268519</v>
-      </c>
-      <c r="Q17" s="27" t="n">
-        <f aca="false">I17/M17</f>
-        <v>0.170176188151042</v>
-      </c>
-      <c r="R17" s="12" t="n">
-        <f aca="false">AVERAGE(O17:Q17)</f>
-        <v>0.183585084514854</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G18" s="0" t="n">
-        <v>10093</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <v>20553</v>
-      </c>
-      <c r="I18" s="0" t="n">
-        <v>36533</v>
-      </c>
-      <c r="K18" s="0" t="n">
-        <f aca="false">A7*B7*C7*D7*D8</f>
+      <c r="N19" s="28" t="n">
+        <f aca="false">F19/J19</f>
+        <v>0.225830078125</v>
+      </c>
+      <c r="O19" s="28" t="n">
+        <f aca="false">G19/K19</f>
+        <v>0.210991753472222</v>
+      </c>
+      <c r="P19" s="28" t="n">
+        <f aca="false">H19/L19</f>
+        <v>0.207183837890625</v>
+      </c>
+      <c r="Q19" s="12" t="n">
+        <f aca="false">AVERAGE(N19:P19)</f>
+        <v>0.214668556495949</v>
+      </c>
+      <c r="R19" s="12" t="n">
+        <f aca="false">AVERAGE(Q16:Q19)</f>
+        <v>0.190784619178301</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="22" t="n">
+        <v>4037</v>
+      </c>
+      <c r="G20" s="22" t="n">
+        <v>8456</v>
+      </c>
+      <c r="H20" s="22" t="n">
+        <v>14500</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <f aca="false">A9*B9*C9*C10</f>
+        <v>12288</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <f aca="false">A9*B9*D9*D10</f>
+        <v>27648</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <f aca="false">A9*B9*E9*E10</f>
         <v>49152</v>
       </c>
-      <c r="L18" s="0" t="n">
-        <f aca="false">A7*B7*C7*E7*E8</f>
-        <v>110592</v>
-      </c>
-      <c r="M18" s="0" t="n">
-        <f aca="false">A7*B7*C7*F7*F8</f>
-        <v>196608</v>
-      </c>
-      <c r="O18" s="27" t="n">
-        <f aca="false">G18/K18</f>
-        <v>0.205342610677083</v>
-      </c>
-      <c r="P18" s="27" t="n">
-        <f aca="false">H18/L18</f>
-        <v>0.185845269097222</v>
-      </c>
-      <c r="Q18" s="27" t="n">
-        <f aca="false">I18/M18</f>
-        <v>0.185816446940104</v>
-      </c>
-      <c r="R18" s="12" t="n">
-        <f aca="false">AVERAGE(O18:Q18)</f>
-        <v>0.19233477557147</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G19" s="0" t="n">
-        <v>5550</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <v>11667</v>
-      </c>
-      <c r="I19" s="0" t="n">
-        <v>20367</v>
-      </c>
-      <c r="K19" s="0" t="n">
-        <f aca="false">A8*B8*C8*D8*D9</f>
-        <v>24576</v>
-      </c>
-      <c r="L19" s="0" t="n">
-        <f aca="false">A8*B8*C8*E8*E9</f>
-        <v>55296</v>
-      </c>
-      <c r="M19" s="0" t="n">
-        <f aca="false">A8*B8*C8*F8*F9</f>
-        <v>98304</v>
-      </c>
-      <c r="O19" s="27" t="n">
-        <f aca="false">G19/K19</f>
-        <v>0.225830078125</v>
-      </c>
-      <c r="P19" s="27" t="n">
-        <f aca="false">H19/L19</f>
-        <v>0.210991753472222</v>
-      </c>
-      <c r="Q19" s="27" t="n">
-        <f aca="false">I19/M19</f>
-        <v>0.207183837890625</v>
-      </c>
-      <c r="R19" s="12" t="n">
-        <f aca="false">AVERAGE(O19:Q19)</f>
-        <v>0.214668556495949</v>
-      </c>
-      <c r="S19" s="12" t="n">
-        <f aca="false">AVERAGE(R16:R19)</f>
-        <v>0.190784619178301</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G20" s="0" t="n">
-        <v>4037</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <v>8456</v>
-      </c>
-      <c r="I20" s="0" t="n">
-        <v>14500</v>
-      </c>
-      <c r="K20" s="0" t="n">
-        <f aca="false">A9*B9*C9*D9*D10</f>
+      <c r="N20" s="29" t="n">
+        <f aca="false">F20/J20</f>
+        <v>0.328531901041667</v>
+      </c>
+      <c r="O20" s="29" t="n">
+        <f aca="false">G20/K20</f>
+        <v>0.305844907407407</v>
+      </c>
+      <c r="P20" s="29" t="n">
+        <f aca="false">H20/L20</f>
+        <v>0.295003255208333</v>
+      </c>
+      <c r="Q20" s="12" t="n">
+        <f aca="false">AVERAGE(N20:P20)</f>
+        <v>0.309793354552469</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F21" s="22" t="n">
+        <v>4283</v>
+      </c>
+      <c r="G21" s="22" t="n">
+        <v>8992</v>
+      </c>
+      <c r="H21" s="22" t="n">
+        <v>15443</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <f aca="false">A10*B10*C10*C11</f>
         <v>12288</v>
       </c>
-      <c r="L20" s="0" t="n">
-        <f aca="false">A9*B9*C9*E9*E10</f>
+      <c r="K21" s="0" t="n">
+        <f aca="false">A10*B10*D10*D11</f>
         <v>27648</v>
       </c>
-      <c r="M20" s="0" t="n">
-        <f aca="false">A9*B9*C9*F9*F10</f>
+      <c r="L21" s="0" t="n">
+        <f aca="false">A10*B10*E10*E11</f>
         <v>49152</v>
       </c>
-      <c r="O20" s="28" t="n">
-        <f aca="false">G20/K20</f>
-        <v>0.328531901041667</v>
-      </c>
-      <c r="P20" s="28" t="n">
-        <f aca="false">H20/L20</f>
-        <v>0.305844907407407</v>
-      </c>
-      <c r="Q20" s="28" t="n">
-        <f aca="false">I20/M20</f>
-        <v>0.295003255208333</v>
-      </c>
-      <c r="R20" s="12" t="n">
-        <f aca="false">AVERAGE(O20:Q20)</f>
-        <v>0.309793354552469</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G21" s="0" t="n">
-        <v>4283</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <v>8992</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>15443</v>
-      </c>
-      <c r="K21" s="0" t="n">
-        <f aca="false">A10*B10*C10*D10*D11</f>
-        <v>12288</v>
-      </c>
-      <c r="L21" s="0" t="n">
-        <f aca="false">A10*B10*C10*E10*E11</f>
-        <v>27648</v>
-      </c>
-      <c r="M21" s="0" t="n">
-        <f aca="false">A10*B10*C10*F10*F11</f>
-        <v>49152</v>
-      </c>
-      <c r="O21" s="28" t="n">
+      <c r="N21" s="29" t="n">
+        <f aca="false">F21/J21</f>
+        <v>0.348551432291667</v>
+      </c>
+      <c r="O21" s="29" t="n">
         <f aca="false">G21/K21</f>
-        <v>0.348551432291667</v>
-      </c>
-      <c r="P21" s="28" t="n">
+        <v>0.325231481481481</v>
+      </c>
+      <c r="P21" s="29" t="n">
         <f aca="false">H21/L21</f>
-        <v>0.325231481481481</v>
-      </c>
-      <c r="Q21" s="28" t="n">
-        <f aca="false">I21/M21</f>
         <v>0.314188639322917</v>
       </c>
+      <c r="Q21" s="12" t="n">
+        <f aca="false">AVERAGE(N21:P21)</f>
+        <v>0.329323851032022</v>
+      </c>
       <c r="R21" s="12" t="n">
-        <f aca="false">AVERAGE(O21:Q21)</f>
-        <v>0.329323851032022</v>
-      </c>
-      <c r="S21" s="12" t="n">
-        <f aca="false">AVERAGE(Q20:Q21)</f>
+        <f aca="false">AVERAGE(P20:P21)</f>
         <v>0.304595947265625</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="19" t="n">
+        <f aca="false">SUM(F15:F21)</f>
+        <v>84986</v>
+      </c>
+      <c r="G22" s="19" t="n">
+        <f aca="false">SUM(G15:G21)</f>
+        <v>169507</v>
+      </c>
+      <c r="H22" s="19" t="n">
+        <f aca="false">SUM(H15:H21)</f>
+        <v>281934</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="C3:E3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>